<commit_message>
Accenture Debug for next link
</commit_message>
<xml_diff>
--- a/Multi_Accenture/accenture_job_data.xlsx
+++ b/Multi_Accenture/accenture_job_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,21 @@
           <t>Experience Required</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Page</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Index</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Industry X- Engineering Digitization &amp; PLM Consultant</t>
+          <t>Workday Certified Integrations Lead- Education &amp; Government</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,19 +478,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Team Lead/Consultant</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager Tech Strategy &amp; Advisory</t>
+          <t>Workday Certified Technical Manager - Education &amp; Government</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,19 +506,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager</t>
+          <t>Business Architecture Manager</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Senior Level</t>
         </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>*Data Management - 5447889</t>
+          <t>Workday Certified Integration Developer Consultant - Education/Government</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,63 +534,81 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Python - Application Developer with Capital Market Experience</t>
+          <t>Workday Certified Data Consultant</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Python - Application Developer- 5333681</t>
+          <t>Workday Certified Financials FDM Lead – Education &amp; Government</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Industry X - Engineering Digitization &amp; PLM Manager</t>
+          <t>Workday Certified Financials R2R Consultant – Education &amp; Government</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,41 +618,53 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Python + Linux Application Developer- 5375070</t>
+          <t>Workday Certified Prism Lead - Education &amp; Government</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Security Account Lead- Healthcare and Public Services Industry</t>
+          <t>Workday Financials Adaptive Consultant – Education &amp; Govt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -622,19 +674,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Security Consulting Senior Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Workday Certified HCM Security Consultant</t>
+          <t>Workday Certified Student Records/Curriculum/Advising Lead - Higher Education</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -644,63 +702,81 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Business Architecture Team Lead/Consultant</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Business Advisory Specialist</t>
+          <t>^Full Stack JAVA Developer - 5467547</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Walnut Creek, CA</t>
+          <t>Florham Park, NJ</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Business Advisory Senior Analyst</t>
+          <t>Software Development Senior Analyst</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>^Project Manager - 5432190</t>
+          <t>^ETL Database Engineer  5411332</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Bloomington, IL</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Program and Project Management Senior Analyst</t>
+          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Full Stack Engineer</t>
+          <t>Consulting Summer Analyst - NAELFY25</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -710,19 +786,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Custom Software Engineering Team Lead/Consultant</t>
+          <t>Mgmt Consulting Analyst</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Early Career</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Industry X- Engineering Digitization &amp; PLM Consultant</t>
+          <t>Technology Summer Analyst - NAELFY25</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -732,19 +814,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Team Lead/Consultant</t>
+          <t>Business Architecture Analyst</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Early Career</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager Tech Strategy &amp; Advisory</t>
+          <t>Oracle Utilities Consultant - Technical Designer</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -754,19 +842,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>*Data Management - 5447889</t>
+          <t>Execution Engineer</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -776,19 +870,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
+          <t>Data Eng, Mgmt &amp; Governance Associate</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Python - Application Developer with Capital Market Experience</t>
+          <t>Splunk Application Developer</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -798,85 +898,109 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Advanced App/Cloud Support &amp; Engineering Analyst</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Python - Application Developer- 5333681</t>
+          <t>Systems Engineering- 5444434</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Florham Park, NJ</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Infra Managed Service Senior Analyst</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Industry X - Engineering Digitization &amp; PLM Manager</t>
+          <t>Ansible Application Developer/Solution Engineer- 5444417</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Various locations</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Manager</t>
+          <t>Advanced App/Cloud Support &amp; Engineering Senior Analyst</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Python + Linux Application Developer- 5375070</t>
+          <t>Oracle GenAI Senior Manager</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Senior Manager</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Senior Level</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Security Account Lead- Healthcare and Public Services Industry</t>
+          <t>Oracle Platform Security Manager</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -893,12 +1017,18 @@
         <is>
           <t>Senior Level</t>
         </is>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Workday Certified HCM Security Consultant</t>
+          <t>Oracle SQL/ PLSQL Lead Developer - 5384983</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -908,63 +1038,81 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Business Architecture Team Lead/Consultant</t>
+          <t>Database Administration Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Business Advisory Specialist</t>
+          <t>SAP JVA/PRA Lead</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Walnut Creek, CA</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Business Advisory Senior Analyst</t>
+          <t>Technology Consulting Manager</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Senior Level</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>^Project Manager - 5432190</t>
+          <t>SAP ABAP Cloud for S/4HANA Developer</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Program and Project Management Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Full Stack Engineer</t>
+          <t>SAP BTP Consultant</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -974,19 +1122,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Custom Software Engineering Team Lead/Consultant</t>
+          <t>Technology Consulting Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Industry X- Engineering Digitization &amp; PLM Consultant</t>
+          <t>Workday Certified Integrations Lead- Education &amp; Government</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -996,19 +1150,25 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Team Lead/Consultant</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager Tech Strategy &amp; Advisory</t>
+          <t>Workday Certified Technical Manager - Education &amp; Government</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1018,19 +1178,25 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager</t>
+          <t>Business Architecture Manager</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>Senior Level</t>
         </is>
+      </c>
+      <c r="E27" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>*Data Management - 5447889</t>
+          <t>Workday Certified Integration Developer Consultant - Education/Government</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1040,63 +1206,81 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Python - Application Developer with Capital Market Experience</t>
+          <t>Workday Certified Data Consultant</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E29" t="n">
+        <v>3</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Python - Application Developer- 5333681</t>
+          <t>Workday Certified Financials FDM Lead – Education &amp; Government</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E30" t="n">
+        <v>3</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Industry X - Engineering Digitization &amp; PLM Manager</t>
+          <t>Workday Certified Financials R2R Consultant – Education &amp; Government</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1106,41 +1290,53 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Python + Linux Application Developer- 5375070</t>
+          <t>Workday Certified Prism Lead - Education &amp; Government</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Security Account Lead- Healthcare and Public Services Industry</t>
+          <t>Workday Financials Adaptive Consultant – Education &amp; Govt</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1150,19 +1346,25 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Security Consulting Senior Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>3</v>
+      </c>
+      <c r="F33" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Workday Certified HCM Security Consultant</t>
+          <t>Workday Certified Student Records/Curriculum/Advising Lead - Higher Education</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1172,63 +1374,81 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Business Architecture Team Lead/Consultant</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Business Advisory Specialist</t>
+          <t>^Full Stack JAVA Developer - 5467547</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Walnut Creek, CA</t>
+          <t>Florham Park, NJ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Business Advisory Senior Analyst</t>
+          <t>Software Development Senior Analyst</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E35" t="n">
+        <v>3</v>
+      </c>
+      <c r="F35" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>^Project Manager - 5432190</t>
+          <t>^ETL Database Engineer  5411332</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Bloomington, IL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Program and Project Management Senior Analyst</t>
+          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E36" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Full Stack Engineer</t>
+          <t>Consulting Summer Analyst - NAELFY25</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1238,19 +1458,25 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Custom Software Engineering Team Lead/Consultant</t>
+          <t>Mgmt Consulting Analyst</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Early Career</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>3</v>
+      </c>
+      <c r="F37" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Industry X- Engineering Digitization &amp; PLM Consultant</t>
+          <t>Technology Summer Analyst - NAELFY25</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1260,19 +1486,25 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Team Lead/Consultant</t>
+          <t>Business Architecture Analyst</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Early Career</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>4</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager Tech Strategy &amp; Advisory</t>
+          <t>Oracle Utilities Consultant - Technical Designer</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1282,19 +1514,25 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>4</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>*Data Management - 5447889</t>
+          <t>Execution Engineer</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1304,19 +1542,25 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
+          <t>Data Eng, Mgmt &amp; Governance Associate</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E40" t="n">
+        <v>4</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Python - Application Developer with Capital Market Experience</t>
+          <t>Splunk Application Developer</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1326,85 +1570,109 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Advanced App/Cloud Support &amp; Engineering Analyst</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Python - Application Developer- 5333681</t>
+          <t>Systems Engineering- 5444434</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Florham Park, NJ</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Infra Managed Service Senior Analyst</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E42" t="n">
+        <v>4</v>
+      </c>
+      <c r="F42" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Industry X - Engineering Digitization &amp; PLM Manager</t>
+          <t>Ansible Application Developer/Solution Engineer- 5444417</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Various locations</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Manager</t>
+          <t>Advanced App/Cloud Support &amp; Engineering Senior Analyst</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>4</v>
+      </c>
+      <c r="F43" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Python + Linux Application Developer- 5375070</t>
+          <t>Oracle GenAI Senior Manager</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Senior Manager</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Senior Level</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>4</v>
+      </c>
+      <c r="F44" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Security Account Lead- Healthcare and Public Services Industry</t>
+          <t>Oracle Platform Security Manager</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1421,12 +1689,18 @@
         <is>
           <t>Senior Level</t>
         </is>
+      </c>
+      <c r="E45" t="n">
+        <v>4</v>
+      </c>
+      <c r="F45" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Workday Certified HCM Security Consultant</t>
+          <t>Oracle SQL/ PLSQL Lead Developer - 5384983</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1436,63 +1710,81 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Business Architecture Team Lead/Consultant</t>
+          <t>Database Administration Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E46" t="n">
+        <v>4</v>
+      </c>
+      <c r="F46" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Business Advisory Specialist</t>
+          <t>SAP JVA/PRA Lead</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Walnut Creek, CA</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Business Advisory Senior Analyst</t>
+          <t>Technology Consulting Manager</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Senior Level</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>4</v>
+      </c>
+      <c r="F47" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>^Project Manager - 5432190</t>
+          <t>SAP ABAP Cloud for S/4HANA Developer</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Program and Project Management Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E48" t="n">
+        <v>4</v>
+      </c>
+      <c r="F48" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Full Stack Engineer</t>
+          <t>SAP BTP Consultant</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1502,19 +1794,25 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Custom Software Engineering Team Lead/Consultant</t>
+          <t>Technology Consulting Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E49" t="n">
+        <v>4</v>
+      </c>
+      <c r="F49" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Industry X- Engineering Digitization &amp; PLM Consultant</t>
+          <t>Workday Certified Integrations Lead- Education &amp; Government</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1524,19 +1822,25 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Team Lead/Consultant</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E50" t="n">
+        <v>5</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager Tech Strategy &amp; Advisory</t>
+          <t>Workday Certified Technical Manager - Education &amp; Government</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1546,19 +1850,25 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Topic Advisory Manager</t>
+          <t>Business Architecture Manager</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>Senior Level</t>
         </is>
+      </c>
+      <c r="E51" t="n">
+        <v>5</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>*Data Management - 5447889</t>
+          <t>Workday Certified Integration Developer Consultant - Education/Government</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1568,63 +1878,81 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E52" t="n">
+        <v>5</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Python - Application Developer with Capital Market Experience</t>
+          <t>Workday Certified Data Consultant</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E53" t="n">
+        <v>5</v>
+      </c>
+      <c r="F53" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Python - Application Developer- 5333681</t>
+          <t>Workday Certified Financials FDM Lead – Education &amp; Government</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E54" t="n">
+        <v>5</v>
+      </c>
+      <c r="F54" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Industry X - Engineering Digitization &amp; PLM Manager</t>
+          <t>Workday Certified Financials R2R Consultant – Education &amp; Government</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1634,41 +1962,53 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Engineering Digitization &amp; PLM Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>5</v>
+      </c>
+      <c r="F55" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Python + Linux Application Developer- 5375070</t>
+          <t>Workday Certified Prism Lead - Education &amp; Government</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Irving, TX</t>
+          <t>Various locations</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Software Development Senior Analyst</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E56" t="n">
+        <v>5</v>
+      </c>
+      <c r="F56" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Security Account Lead- Healthcare and Public Services Industry</t>
+          <t>Workday Financials Adaptive Consultant – Education &amp; Govt</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1678,19 +2018,25 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Security Consulting Senior Manager</t>
+          <t>Business Architecture Team Lead/Consultant</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Senior Level</t>
-        </is>
+          <t>Mid-Level</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>5</v>
+      </c>
+      <c r="F57" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Workday Certified HCM Security Consultant</t>
+          <t>Workday Certified Student Records/Curriculum/Advising Lead - Higher Education</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1700,63 +2046,81 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Business Architecture Team Lead/Consultant</t>
+          <t>Business Architecture Associate Manager</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E58" t="n">
+        <v>5</v>
+      </c>
+      <c r="F58" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Business Advisory Specialist</t>
+          <t>^Full Stack JAVA Developer - 5467547</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Walnut Creek, CA</t>
+          <t>Florham Park, NJ</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Business Advisory Senior Analyst</t>
+          <t>Software Development Senior Analyst</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E59" t="n">
+        <v>5</v>
+      </c>
+      <c r="F59" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>^Project Manager - 5432190</t>
+          <t>^ETL Database Engineer  5411332</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Bloomington, IL</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Program and Project Management Senior Analyst</t>
+          <t>Data Eng, Mgmt &amp; Governance Senior Analyst</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
           <t>Mid-Level</t>
         </is>
+      </c>
+      <c r="E60" t="n">
+        <v>5</v>
+      </c>
+      <c r="F60" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Full Stack Engineer</t>
+          <t>Consulting Summer Analyst - NAELFY25</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1766,13 +2130,19 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Custom Software Engineering Team Lead/Consultant</t>
+          <t>Mgmt Consulting Analyst</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Mid-Level</t>
-        </is>
+          <t>Early Career</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>5</v>
+      </c>
+      <c r="F61" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>